<commit_message>
Readme and sprints finalized
</commit_message>
<xml_diff>
--- a/Documents/Sprints/December sprint.xlsx
+++ b/Documents/Sprints/December sprint.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="270" yWindow="630" windowWidth="24615" windowHeight="11445"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -88,80 +91,52 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
     </font>
@@ -171,9 +146,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -407,309 +380,603 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="1" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="3" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="2">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="5" applyFont="1" fontId="3">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="6" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="4">
-      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="3" xfId="0" numFmtId="0" borderId="8" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="9" applyFont="1" fontId="5">
-      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="10" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="11" fontId="0">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="0" xfId="0" numFmtId="164" borderId="12" applyFont="1" fontId="6" applyNumberFormat="1">
-      <alignment vertical="bottom" horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="4" xfId="0" numFmtId="0" borderId="13" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="14" applyFont="1" fontId="7" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" applyAlignment="1" fillId="6" xfId="0" numFmtId="0" borderId="15" fontId="0" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.14" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" customWidth="1" max="5" width="35.71"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c s="14" r="A1"/>
-      <c t="s" s="4" r="B1">
+    <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c s="13" r="A2"/>
-      <c t="s" s="4" r="B2">
+    <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10"/>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c s="15" r="A3"/>
-      <c t="s" s="4" r="B3">
+    <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4">
-      <c s="6" r="A4"/>
-    </row>
-    <row r="5">
-      <c s="11" r="A5"/>
-      <c s="11" r="B5"/>
-      <c t="s" s="7" r="C5">
+    <row r="4" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
-      <c s="7" r="D5"/>
-      <c s="7" r="E5"/>
-    </row>
-    <row r="6">
-      <c t="s" s="5" r="A6">
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="5" r="B6">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c s="12" r="C6">
+      <c r="C6" s="14">
         <v>41225</v>
       </c>
-      <c s="9" r="D6"/>
-      <c s="9" r="E6"/>
-      <c s="1" r="F6"/>
-    </row>
-    <row r="7">
-      <c t="s" s="3" r="A7">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="3" r="B7">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C7">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="D7">
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="15" r="E7">
+      <c r="E7" s="12" t="s">
         <v>10</v>
       </c>
-      <c s="1" r="F7"/>
-    </row>
-    <row r="8">
-      <c t="s" s="3" r="A8">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="3" r="B8">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C8">
+      <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="D8">
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="15" r="E8">
+      <c r="E8" s="12" t="s">
         <v>13</v>
       </c>
-      <c s="1" r="F8"/>
-    </row>
-    <row r="9">
-      <c t="s" s="3" r="A9">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="3" r="B9">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C9">
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="D9">
+      <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="15" r="E9">
+      <c r="E9" s="12" t="s">
         <v>13</v>
       </c>
-      <c s="1" r="F9"/>
-    </row>
-    <row r="10">
-      <c t="s" s="3" r="A10">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="3" r="B10">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C10">
+      <c r="C10" s="7" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="D10">
+      <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="15" r="E10">
+      <c r="E10" s="12" t="s">
         <v>13</v>
       </c>
-      <c s="1" r="F10"/>
-    </row>
-    <row r="11">
-      <c t="s" s="3" r="A11">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="3" r="B11">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C11">
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="D11">
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="15" r="E11">
+      <c r="E11" s="12" t="s">
         <v>18</v>
       </c>
-      <c s="1" r="F11"/>
-    </row>
-    <row r="12">
-      <c t="s" s="3" r="A12">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="3" r="B12">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C12">
+      <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="D12">
+      <c r="D12" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="15" r="E12">
+      <c r="E12" s="12" t="s">
         <v>18</v>
       </c>
-      <c s="1" r="F12"/>
-    </row>
-    <row r="13">
-      <c t="s" s="3" r="A13">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="3" r="B13">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C13">
+      <c r="C13" s="7" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="D13">
+      <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="15" r="E13">
+      <c r="E13" s="12" t="s">
         <v>13</v>
       </c>
-      <c s="1" r="F13"/>
-    </row>
-    <row r="14">
-      <c t="s" s="3" r="A14">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="3" r="B14">
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C14">
+      <c r="C14" s="7" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="2" r="D14">
+      <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="s" s="15" r="E14">
+      <c r="E14" s="12" t="s">
         <v>13</v>
       </c>
-      <c s="1" r="F14"/>
-    </row>
-    <row r="15">
-      <c t="s" s="3" r="A15">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c t="s" s="3" r="B15">
+      <c r="B15" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C15">
+      <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="D15">
+      <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="15" r="E15">
+      <c r="E15" s="12" t="s">
         <v>18</v>
       </c>
-      <c s="1" r="F15"/>
-    </row>
-    <row r="16">
-      <c t="s" s="3" r="A16">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="3" r="B16">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="8" r="C16">
+      <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="D16">
+      <c r="D16" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="15" r="E16">
+      <c r="E16" s="12" t="s">
         <v>18</v>
       </c>
-      <c s="1" r="F16"/>
-    </row>
-    <row r="17">
-      <c s="6" r="A17"/>
-      <c s="10" r="B17"/>
-      <c s="10" r="C17"/>
-      <c s="10" r="D17"/>
-      <c s="10" r="E17"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C6:E6"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>